<commit_message>
changes to the sample metadata sheet continaing the custom fields, for testing purposes
</commit_message>
<xml_diff>
--- a/assets/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankushkgupta\Documents\CDC\tostadas-deloitte\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ufl1\Desktop\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1151BC2-DF47-4FC7-967B-DF1C0720F6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C9559C4-CD72-462B-AF47-07B57FBC599A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5600" yWindow="3290" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPXV_Metadata" sheetId="6" r:id="rId1"/>
@@ -2862,7 +2862,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="425">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4122,6 +4122,21 @@
   </si>
   <si>
     <t>host</t>
+  </si>
+  <si>
+    <t>test_field_1</t>
+  </si>
+  <si>
+    <t>test_field_2</t>
+  </si>
+  <si>
+    <t>test_field_3</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -4809,14 +4824,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5249,34 +5264,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB79B10-5F4B-4CF2-A235-6BD3FDFF8F8F}">
-  <dimension ref="A1:AK46"/>
+  <dimension ref="A1:AO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.453125" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" customWidth="1"/>
+    <col min="22" max="22" width="24.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>321</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
       <c r="O1" s="28" t="s">
         <v>320</v>
       </c>
@@ -5293,7 +5308,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:41">
       <c r="A2" s="18" t="s">
         <v>413</v>
       </c>
@@ -5306,10 +5321,10 @@
       <c r="D2" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>418</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>419</v>
       </c>
       <c r="G2" s="18" t="s">
@@ -5405,8 +5420,17 @@
       <c r="AK2" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:37">
+      <c r="AM2" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="AN2" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="AO2" s="18" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>372</v>
       </c>
@@ -5469,8 +5493,17 @@
         <v>402</v>
       </c>
       <c r="AE3" s="28"/>
-    </row>
-    <row r="4" spans="1:37">
+      <c r="AM3">
+        <v>2</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>424</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41">
       <c r="A4" t="s">
         <v>373</v>
       </c>
@@ -5530,8 +5563,17 @@
         <v>404</v>
       </c>
       <c r="AE4" s="28"/>
-    </row>
-    <row r="5" spans="1:37">
+      <c r="AM4">
+        <v>5</v>
+      </c>
+      <c r="AN4">
+        <v>3.5</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41">
       <c r="A5" t="s">
         <v>374</v>
       </c>
@@ -5591,8 +5633,17 @@
         <v>406</v>
       </c>
       <c r="AE5" s="28"/>
-    </row>
-    <row r="6" spans="1:37">
+      <c r="AM5">
+        <v>8</v>
+      </c>
+      <c r="AN5">
+        <v>3</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41">
       <c r="A6" t="s">
         <v>375</v>
       </c>
@@ -5655,8 +5706,17 @@
         <v>408</v>
       </c>
       <c r="AE6" s="28"/>
-    </row>
-    <row r="7" spans="1:37">
+      <c r="AM6">
+        <v>4</v>
+      </c>
+      <c r="AN6">
+        <v>3.2</v>
+      </c>
+      <c r="AO6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41">
       <c r="A7" t="s">
         <v>376</v>
       </c>
@@ -5719,8 +5779,17 @@
         <v>410</v>
       </c>
       <c r="AE7" s="28"/>
-    </row>
-    <row r="8" spans="1:37">
+      <c r="AM7" t="s">
+        <v>423</v>
+      </c>
+      <c r="AN7">
+        <v>1.5</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41">
       <c r="A8" t="s">
         <v>411</v>
       </c>
@@ -5783,8 +5852,17 @@
         <v>410</v>
       </c>
       <c r="AE8" s="28"/>
-    </row>
-    <row r="9" spans="1:37">
+      <c r="AM8">
+        <v>3</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41">
       <c r="A9" t="s">
         <v>412</v>
       </c>
@@ -5847,71 +5925,74 @@
         <v>410</v>
       </c>
       <c r="AE9" s="28"/>
-    </row>
-    <row r="10" spans="1:37">
+      <c r="AM9" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41">
       <c r="D10" s="28"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
       <c r="O10" s="28"/>
       <c r="S10" s="28"/>
       <c r="V10" s="28"/>
       <c r="W10" s="28"/>
       <c r="AE10" s="28"/>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:41">
       <c r="D11" s="28"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
       <c r="O11" s="28"/>
       <c r="S11" s="28"/>
       <c r="V11" s="28"/>
       <c r="W11" s="28"/>
       <c r="AE11" s="28"/>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:41">
       <c r="D12" s="28"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
       <c r="O12" s="28"/>
       <c r="S12" s="28"/>
       <c r="V12" s="28"/>
       <c r="W12" s="28"/>
       <c r="AE12" s="28"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:41">
       <c r="D13" s="28"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="O13" s="28"/>
       <c r="S13" s="28"/>
       <c r="V13" s="28"/>
       <c r="W13" s="28"/>
       <c r="AE13" s="28"/>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:41">
       <c r="D14" s="28"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
       <c r="O14" s="28"/>
       <c r="S14" s="28"/>
       <c r="V14" s="28"/>
       <c r="W14" s="28"/>
       <c r="AE14" s="28"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:41">
       <c r="D15" s="28"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
       <c r="O15" s="28"/>
       <c r="S15" s="28"/>
       <c r="V15" s="28"/>
       <c r="W15" s="28"/>
       <c r="AE15" s="28"/>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:41">
       <c r="D16" s="28"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
       <c r="O16" s="28"/>
       <c r="S16" s="28"/>
       <c r="V16" s="28"/>
@@ -5920,8 +6001,8 @@
     </row>
     <row r="17" spans="4:31">
       <c r="D17" s="28"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
       <c r="O17" s="28"/>
       <c r="S17" s="28"/>
       <c r="V17" s="28"/>
@@ -5930,8 +6011,8 @@
     </row>
     <row r="18" spans="4:31">
       <c r="D18" s="28"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
       <c r="O18" s="28"/>
       <c r="S18" s="28"/>
       <c r="V18" s="28"/>
@@ -5940,8 +6021,8 @@
     </row>
     <row r="19" spans="4:31">
       <c r="D19" s="28"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
       <c r="O19" s="28"/>
       <c r="S19" s="28"/>
       <c r="V19" s="28"/>
@@ -5950,8 +6031,8 @@
     </row>
     <row r="20" spans="4:31">
       <c r="D20" s="28"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
       <c r="O20" s="28"/>
       <c r="S20" s="28"/>
       <c r="V20" s="28"/>
@@ -5960,8 +6041,8 @@
     </row>
     <row r="21" spans="4:31">
       <c r="D21" s="28"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
       <c r="O21" s="28"/>
       <c r="S21" s="28"/>
       <c r="V21" s="28"/>
@@ -5970,8 +6051,8 @@
     </row>
     <row r="22" spans="4:31">
       <c r="D22" s="28"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
       <c r="O22" s="28"/>
       <c r="S22" s="28"/>
       <c r="V22" s="28"/>
@@ -5980,8 +6061,8 @@
     </row>
     <row r="23" spans="4:31">
       <c r="D23" s="28"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
       <c r="O23" s="28"/>
       <c r="S23" s="28"/>
       <c r="V23" s="28"/>
@@ -5990,8 +6071,8 @@
     </row>
     <row r="24" spans="4:31">
       <c r="D24" s="28"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
       <c r="O24" s="28"/>
       <c r="S24" s="28"/>
       <c r="V24" s="28"/>
@@ -6000,8 +6081,8 @@
     </row>
     <row r="25" spans="4:31">
       <c r="D25" s="28"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
       <c r="O25" s="28"/>
       <c r="S25" s="28"/>
       <c r="V25" s="28"/>
@@ -6010,8 +6091,8 @@
     </row>
     <row r="26" spans="4:31">
       <c r="D26" s="28"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
       <c r="O26" s="28"/>
       <c r="S26" s="28"/>
       <c r="V26" s="28"/>
@@ -6020,8 +6101,8 @@
     </row>
     <row r="27" spans="4:31">
       <c r="D27" s="28"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
       <c r="O27" s="28"/>
       <c r="S27" s="28"/>
       <c r="V27" s="28"/>
@@ -6030,8 +6111,8 @@
     </row>
     <row r="28" spans="4:31">
       <c r="D28" s="28"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
       <c r="O28" s="28"/>
       <c r="S28" s="28"/>
       <c r="V28" s="28"/>
@@ -6040,8 +6121,8 @@
     </row>
     <row r="29" spans="4:31">
       <c r="D29" s="28"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
       <c r="O29" s="28"/>
       <c r="S29" s="28"/>
       <c r="V29" s="28"/>
@@ -6050,8 +6131,8 @@
     </row>
     <row r="30" spans="4:31">
       <c r="D30" s="28"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
       <c r="O30" s="28"/>
       <c r="S30" s="28"/>
       <c r="V30" s="28"/>
@@ -6060,8 +6141,8 @@
     </row>
     <row r="31" spans="4:31">
       <c r="D31" s="28"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
       <c r="O31" s="28"/>
       <c r="S31" s="28"/>
       <c r="V31" s="28"/>
@@ -6070,8 +6151,8 @@
     </row>
     <row r="32" spans="4:31">
       <c r="D32" s="28"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
       <c r="O32" s="28"/>
       <c r="S32" s="28"/>
       <c r="V32" s="28"/>
@@ -6080,8 +6161,8 @@
     </row>
     <row r="33" spans="4:31">
       <c r="D33" s="28"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
       <c r="O33" s="28"/>
       <c r="S33" s="28"/>
       <c r="V33" s="28"/>
@@ -6090,8 +6171,8 @@
     </row>
     <row r="34" spans="4:31">
       <c r="D34" s="28"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
       <c r="O34" s="28"/>
       <c r="S34" s="28"/>
       <c r="V34" s="28"/>
@@ -6100,8 +6181,8 @@
     </row>
     <row r="35" spans="4:31">
       <c r="D35" s="28"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
       <c r="O35" s="28"/>
       <c r="S35" s="28"/>
       <c r="V35" s="28"/>
@@ -6110,8 +6191,8 @@
     </row>
     <row r="36" spans="4:31">
       <c r="D36" s="28"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
       <c r="O36" s="28"/>
       <c r="S36" s="28"/>
       <c r="V36" s="28"/>
@@ -6120,8 +6201,8 @@
     </row>
     <row r="37" spans="4:31">
       <c r="D37" s="28"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="O37" s="28"/>
       <c r="S37" s="28"/>
       <c r="V37" s="28"/>
@@ -6130,8 +6211,8 @@
     </row>
     <row r="38" spans="4:31">
       <c r="D38" s="28"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
       <c r="O38" s="28"/>
       <c r="S38" s="28"/>
       <c r="V38" s="28"/>
@@ -6140,8 +6221,8 @@
     </row>
     <row r="39" spans="4:31">
       <c r="D39" s="28"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
       <c r="O39" s="28"/>
       <c r="S39" s="28"/>
       <c r="V39" s="28"/>
@@ -6150,8 +6231,8 @@
     </row>
     <row r="40" spans="4:31">
       <c r="D40" s="28"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
       <c r="O40" s="28"/>
       <c r="S40" s="28"/>
       <c r="V40" s="28"/>
@@ -6160,8 +6241,8 @@
     </row>
     <row r="41" spans="4:31">
       <c r="D41" s="28"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
       <c r="O41" s="28"/>
       <c r="S41" s="28"/>
       <c r="V41" s="28"/>
@@ -6170,8 +6251,8 @@
     </row>
     <row r="42" spans="4:31">
       <c r="D42" s="28"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
       <c r="O42" s="28"/>
       <c r="S42" s="28"/>
       <c r="V42" s="28"/>
@@ -6180,8 +6261,8 @@
     </row>
     <row r="43" spans="4:31">
       <c r="D43" s="28"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
       <c r="O43" s="28"/>
       <c r="S43" s="28"/>
       <c r="V43" s="28"/>
@@ -6190,8 +6271,8 @@
     </row>
     <row r="44" spans="4:31">
       <c r="D44" s="28"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
       <c r="O44" s="28"/>
       <c r="S44" s="28"/>
       <c r="V44" s="28"/>
@@ -6200,8 +6281,8 @@
     </row>
     <row r="45" spans="4:31">
       <c r="D45" s="28"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
       <c r="O45" s="28"/>
       <c r="S45" s="28"/>
       <c r="V45" s="28"/>
@@ -6210,8 +6291,8 @@
     </row>
     <row r="46" spans="4:31">
       <c r="D46" s="28"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
       <c r="O46" s="28"/>
       <c r="S46" s="28"/>
       <c r="V46" s="28"/>
@@ -6275,17 +6356,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
+    <col min="20" max="20" width="24.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -7257,7 +7338,7 @@
       <c r="U23" s="28"/>
       <c r="AC23" s="28"/>
     </row>
-    <row r="24" spans="1:35" ht="18">
+    <row r="24" spans="1:35" ht="18.5">
       <c r="A24" s="27"/>
       <c r="B24" s="33" t="s">
         <v>363</v>
@@ -7401,29 +7482,29 @@
       <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" thickTop="1" thickBottom="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" thickTop="1" thickBottom="1"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.109375" style="24"/>
+    <col min="1" max="1" width="14.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.08984375" style="24"/>
     <col min="9" max="9" width="13" style="19" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="24"/>
-    <col min="11" max="12" width="9.109375" style="12"/>
-    <col min="13" max="14" width="9.109375" style="23"/>
-    <col min="15" max="15" width="9.109375" style="12"/>
-    <col min="16" max="16" width="14.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" style="19"/>
-    <col min="18" max="19" width="9.109375" style="12"/>
-    <col min="20" max="24" width="9.109375" style="13"/>
-    <col min="25" max="29" width="9.109375" style="14"/>
-    <col min="32" max="32" width="9.109375" style="26"/>
-    <col min="33" max="33" width="23.44140625" customWidth="1"/>
-    <col min="37" max="38" width="9.109375" style="13"/>
-    <col min="39" max="39" width="9.109375" style="14"/>
-    <col min="40" max="40" width="19.77734375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" style="24"/>
+    <col min="11" max="12" width="9.08984375" style="12"/>
+    <col min="13" max="14" width="9.08984375" style="23"/>
+    <col min="15" max="15" width="9.08984375" style="12"/>
+    <col min="16" max="16" width="14.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" style="19"/>
+    <col min="18" max="19" width="9.08984375" style="12"/>
+    <col min="20" max="24" width="9.08984375" style="13"/>
+    <col min="25" max="29" width="9.08984375" style="14"/>
+    <col min="32" max="32" width="9.08984375" style="26"/>
+    <col min="33" max="33" width="23.453125" customWidth="1"/>
+    <col min="37" max="38" width="9.08984375" style="13"/>
+    <col min="39" max="39" width="9.08984375" style="14"/>
+    <col min="40" max="40" width="19.81640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="18" customFormat="1" thickTop="1" thickBot="1">
@@ -7724,10 +7805,10 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -7930,11 +8011,11 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -8142,25 +8223,25 @@
       <selection activeCell="B18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1">
       <c r="A1" s="5"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -8174,10 +8255,10 @@
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -8191,10 +8272,10 @@
       <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -8208,10 +8289,10 @@
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -8225,10 +8306,10 @@
       <c r="A5" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -8242,10 +8323,10 @@
       <c r="A6" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -8259,10 +8340,10 @@
       <c r="A7" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -8276,10 +8357,10 @@
       <c r="A8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -8293,10 +8374,10 @@
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -8310,10 +8391,10 @@
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -8327,10 +8408,10 @@
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -8344,10 +8425,10 @@
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -8361,10 +8442,10 @@
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -8378,10 +8459,10 @@
       <c r="A14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -8395,10 +8476,10 @@
       <c r="A15" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -8412,10 +8493,10 @@
       <c r="A16" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -8429,10 +8510,10 @@
       <c r="A17" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -8446,10 +8527,10 @@
       <c r="A18" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -8463,10 +8544,10 @@
       <c r="A19" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="35"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -8480,10 +8561,10 @@
       <c r="A20" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="35"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -8497,10 +8578,10 @@
       <c r="A21" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="35"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -8514,10 +8595,10 @@
       <c r="A22" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="35"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -8531,10 +8612,10 @@
       <c r="A23" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="35"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -8548,10 +8629,10 @@
       <c r="A24" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="35"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -8761,10 +8842,10 @@
       <c r="A37" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="35"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -8776,8 +8857,8 @@
     </row>
     <row r="38" spans="1:11" ht="15" thickBot="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -8791,10 +8872,10 @@
       <c r="A39" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="36"/>
+      <c r="C39" s="38"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -8808,10 +8889,10 @@
       <c r="A40" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="35"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -8825,10 +8906,10 @@
       <c r="A41" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="C41" s="35"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -8842,10 +8923,10 @@
       <c r="A42" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="35"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -8859,10 +8940,10 @@
       <c r="A43" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="35"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -8876,10 +8957,10 @@
       <c r="A44" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C44" s="35"/>
+      <c r="C44" s="37"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -8893,10 +8974,10 @@
       <c r="A45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="35"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -8940,10 +9021,10 @@
       <c r="A48" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="C48" s="35"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -8955,8 +9036,8 @@
     </row>
     <row r="49" spans="1:11" ht="15" thickBot="1">
       <c r="A49" s="5"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -8970,10 +9051,10 @@
       <c r="A50" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="35"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -8987,10 +9068,10 @@
       <c r="A51" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="C51" s="35"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -9004,10 +9085,10 @@
       <c r="A52" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="35"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -9021,10 +9102,10 @@
       <c r="A53" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="35"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -9038,10 +9119,10 @@
       <c r="A54" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="C54" s="35"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -9055,10 +9136,10 @@
       <c r="A55" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="C55" s="35"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -9072,10 +9153,10 @@
       <c r="A56" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="35"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -9089,10 +9170,10 @@
       <c r="A57" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="35"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -9106,10 +9187,10 @@
       <c r="A58" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="35"/>
+      <c r="C58" s="37"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -9123,10 +9204,10 @@
       <c r="A59" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="C59" s="35"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -9140,10 +9221,10 @@
       <c r="A60" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="C60" s="35"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -9157,10 +9238,10 @@
       <c r="A61" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="C61" s="35"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
@@ -9174,10 +9255,10 @@
       <c r="A62" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B62" s="35" t="s">
+      <c r="B62" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="C62" s="35"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -9191,10 +9272,10 @@
       <c r="A63" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="35" t="s">
+      <c r="B63" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="C63" s="35"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -9208,10 +9289,10 @@
       <c r="A64" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="C64" s="35"/>
+      <c r="C64" s="37"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
@@ -9225,10 +9306,10 @@
       <c r="A65" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="35"/>
+      <c r="C65" s="37"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -9242,10 +9323,10 @@
       <c r="A66" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B66" s="35" t="s">
+      <c r="B66" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C66" s="35"/>
+      <c r="C66" s="37"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -9259,10 +9340,10 @@
       <c r="A67" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C67" s="35"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -9276,10 +9357,10 @@
       <c r="A68" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="C68" s="35"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
@@ -9293,10 +9374,10 @@
       <c r="A69" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="C69" s="35"/>
+      <c r="C69" s="37"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -9310,10 +9391,10 @@
       <c r="A70" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B70" s="35" t="s">
+      <c r="B70" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="C70" s="35"/>
+      <c r="C70" s="37"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -9327,10 +9408,10 @@
       <c r="A71" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="C71" s="35"/>
+      <c r="C71" s="37"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -9344,10 +9425,10 @@
       <c r="A72" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="C72" s="35"/>
+      <c r="C72" s="37"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -9361,10 +9442,10 @@
       <c r="A73" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="C73" s="35"/>
+      <c r="C73" s="37"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -9378,10 +9459,10 @@
       <c r="A74" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="C74" s="35"/>
+      <c r="C74" s="37"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -9395,10 +9476,10 @@
       <c r="A75" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="C75" s="35"/>
+      <c r="C75" s="37"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -9412,10 +9493,10 @@
       <c r="A76" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B76" s="35" t="s">
+      <c r="B76" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="C76" s="35"/>
+      <c r="C76" s="37"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
@@ -9429,10 +9510,10 @@
       <c r="A77" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="35"/>
+      <c r="C77" s="37"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
@@ -9669,7 +9750,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="26.4">
+    <row r="89" spans="1:11" ht="27.5">
       <c r="A89" s="5" t="s">
         <v>253</v>
       </c>
@@ -9700,7 +9781,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="26.4">
+    <row r="90" spans="1:11" ht="27.5">
       <c r="A90" s="5" t="s">
         <v>250</v>
       </c>
@@ -9729,7 +9810,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="26.4">
+    <row r="91" spans="1:11" ht="27.5">
       <c r="A91" s="5" t="s">
         <v>248</v>
       </c>
@@ -10020,15 +10101,48 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
@@ -10041,48 +10155,15 @@
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>